<commit_message>
updated BoM with motor control info.
</commit_message>
<xml_diff>
--- a/design/AGSE_BOM.xlsx
+++ b/design/AGSE_BOM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Documents\VADL\agse\design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Repos\agse\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Fuse_Board" sheetId="3" r:id="rId2"/>
     <sheet name="Arm_Motor_Controller" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027" iterateDelta="1E-4"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="184">
   <si>
     <t>Manufacturer Number</t>
   </si>
@@ -416,6 +416,168 @@
   </si>
   <si>
     <t>90272A106</t>
+  </si>
+  <si>
+    <t>Motor Control PCB</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ds/2/149/FQP30N06L-244344.pdf</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ds/2/149/FQP27P06-244293.pdf</t>
+  </si>
+  <si>
+    <t>PFET</t>
+  </si>
+  <si>
+    <t>NFET</t>
+  </si>
+  <si>
+    <t>NPN Transisor</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ds/2/302/BC846_SER-840048.pdf</t>
+  </si>
+  <si>
+    <t>5V Regulator</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ds/2/389/CD00001883-310744.pdf</t>
+  </si>
+  <si>
+    <t>LD1085V50</t>
+  </si>
+  <si>
+    <t>PTC for motors</t>
+  </si>
+  <si>
+    <t>MF-SMDF050-2</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ds/2/54/fsmdf2-777754.pdf</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ds/2/427/murs340-240280.pdf</t>
+  </si>
+  <si>
+    <t>MURS360-E3/57T</t>
+  </si>
+  <si>
+    <t>1N4148</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ds/2/149/1N4148-888354.pdf</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ds/2/276/0022436030_PCB_HEADERS-227784.pdf</t>
+  </si>
+  <si>
+    <t>22-43-6030</t>
+  </si>
+  <si>
+    <t>SPOX-3 for AX12A</t>
+  </si>
+  <si>
+    <t>100uF Capacitor</t>
+  </si>
+  <si>
+    <t>UWT1V101MCL1GS</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ds/2/293/e-uwt-880115.pdf</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ds/2/396/mlcc_all_e-541559.pdf</t>
+  </si>
+  <si>
+    <t>10uF Capacitor</t>
+  </si>
+  <si>
+    <t>LMK316B7106KL-TD</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ds/2/281/c02e-2905.pdf</t>
+  </si>
+  <si>
+    <t>0.1uF Capacitor</t>
+  </si>
+  <si>
+    <t>GRM155R61A104KA01D</t>
+  </si>
+  <si>
+    <t>1.7K Resistor</t>
+  </si>
+  <si>
+    <t>3.3K Resistor</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ds/2/427/tnpw_e3-64594.pdf</t>
+  </si>
+  <si>
+    <t>TNPW08051K69BEEA</t>
+  </si>
+  <si>
+    <t>TNPW08053K32BEEA</t>
+  </si>
+  <si>
+    <t>7K Resistor</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ds/2/392/susumu_RR_Data_Sheet-358748.pdf</t>
+  </si>
+  <si>
+    <t>RR1220P-6981-D-M</t>
+  </si>
+  <si>
+    <t>10K Resistor</t>
+  </si>
+  <si>
+    <t>RR1220P-103-D</t>
+  </si>
+  <si>
+    <t>50 Resistor</t>
+  </si>
+  <si>
+    <t>PCF0805-02-49R9DT1</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ds/2/414/PCF-437472.pdf</t>
+  </si>
+  <si>
+    <t>Sparkfun</t>
+  </si>
+  <si>
+    <t>PRT-12620</t>
+  </si>
+  <si>
+    <t>PRT-09918</t>
+  </si>
+  <si>
+    <t>http://www.sparkfun.com/datasheets/Prototyping/2pin_molex_set_19iv10.pdf</t>
+  </si>
+  <si>
+    <t>http://cdn.sparkfun.com/datasheets/Components/LED/S150ANB4.pdf</t>
+  </si>
+  <si>
+    <t>Molex 4 Locking</t>
+  </si>
+  <si>
+    <t>Molex 4 Locking 90deg</t>
+  </si>
+  <si>
+    <t>22-05-3041</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ds/2/276/0022053041_PCB_HEADERS-158631.pdf</t>
+  </si>
+  <si>
+    <t>22-23-2041</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ds/2/276/0022232041_PCB_HEADERS-526511.pdf</t>
+  </si>
+  <si>
+    <t>25 pk</t>
   </si>
 </sst>
 </file>
@@ -649,23 +811,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -701,23 +846,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -870,10 +998,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,7 +1095,7 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H16" si="0">F3*G3</f>
+        <f t="shared" ref="H3:H27" si="0">F3*G3</f>
         <v>6.58</v>
       </c>
       <c r="I3" t="s">
@@ -1062,58 +1190,546 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>130</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F8">
+        <v>1.28</v>
+      </c>
+      <c r="G8">
+        <v>20</v>
+      </c>
       <c r="H8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>25.6</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E9" s="2"/>
+      <c r="A9" t="s">
+        <v>134</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>130</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F9">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="G9">
+        <v>20</v>
+      </c>
       <c r="H9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>22.200000000000003</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>135</v>
+      </c>
+      <c r="B10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
+        <v>130</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F10">
+        <v>0.13</v>
+      </c>
+      <c r="G10">
+        <v>60</v>
+      </c>
       <c r="H10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7.8000000000000007</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B11" t="s">
+        <v>139</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>130</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F11">
+        <v>1.49</v>
+      </c>
+      <c r="G11">
+        <v>8</v>
+      </c>
       <c r="H11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>11.92</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>140</v>
+      </c>
+      <c r="B12" t="s">
+        <v>141</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
+        <v>130</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F12">
+        <v>0.42</v>
+      </c>
+      <c r="G12">
+        <v>16</v>
+      </c>
       <c r="H12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.72</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" t="s">
+        <v>144</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>130</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F13">
+        <v>0.7</v>
+      </c>
+      <c r="G13">
+        <v>10</v>
+      </c>
       <c r="H13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" t="s">
+        <v>145</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" t="s">
+        <v>130</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F14">
+        <v>0.1</v>
+      </c>
+      <c r="G14">
+        <v>10</v>
+      </c>
       <c r="H14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>149</v>
+      </c>
+      <c r="B15" t="s">
+        <v>148</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" t="s">
+        <v>130</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="F15">
+        <v>0.47</v>
+      </c>
+      <c r="G15">
+        <v>15</v>
+      </c>
       <c r="H15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7.05</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>150</v>
+      </c>
+      <c r="B16" t="s">
+        <v>151</v>
+      </c>
+      <c r="C16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" t="s">
+        <v>130</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F16">
+        <v>0.36</v>
+      </c>
+      <c r="G16">
+        <v>15</v>
+      </c>
       <c r="H16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5.3999999999999995</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>154</v>
+      </c>
+      <c r="B17" t="s">
+        <v>155</v>
+      </c>
+      <c r="C17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" t="s">
+        <v>130</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="F17">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G17">
+        <v>15</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>4.3499999999999996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B18" t="s">
+        <v>158</v>
+      </c>
+      <c r="C18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" t="s">
+        <v>130</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F18">
+        <v>0.1</v>
+      </c>
+      <c r="G18">
+        <v>15</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>159</v>
+      </c>
+      <c r="B19" t="s">
+        <v>162</v>
+      </c>
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" t="s">
+        <v>130</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="F19">
+        <v>0.49</v>
+      </c>
+      <c r="G19">
+        <v>30</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>14.7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>160</v>
+      </c>
+      <c r="B20" t="s">
+        <v>163</v>
+      </c>
+      <c r="C20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" t="s">
+        <v>130</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="F20">
+        <v>0.48</v>
+      </c>
+      <c r="G20">
+        <v>30</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>14.399999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>164</v>
+      </c>
+      <c r="B21" t="s">
+        <v>166</v>
+      </c>
+      <c r="C21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" t="s">
+        <v>130</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="F21">
+        <v>0.1</v>
+      </c>
+      <c r="G21">
+        <v>10</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>167</v>
+      </c>
+      <c r="B22" t="s">
+        <v>168</v>
+      </c>
+      <c r="C22" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" t="s">
+        <v>130</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="F22">
+        <v>0.1</v>
+      </c>
+      <c r="G22">
+        <v>25</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>169</v>
+      </c>
+      <c r="B23" t="s">
+        <v>170</v>
+      </c>
+      <c r="C23" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F23">
+        <v>0.1</v>
+      </c>
+      <c r="G23">
+        <v>25</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>177</v>
+      </c>
+      <c r="B24" t="s">
+        <v>181</v>
+      </c>
+      <c r="C24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" t="s">
+        <v>130</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="F24">
+        <v>0.23</v>
+      </c>
+      <c r="G24">
+        <v>10</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="0"/>
+        <v>2.3000000000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>178</v>
+      </c>
+      <c r="B25" t="s">
+        <v>179</v>
+      </c>
+      <c r="C25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" t="s">
+        <v>130</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="F25">
+        <v>0.71</v>
+      </c>
+      <c r="G25">
+        <v>10</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="0"/>
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B26" t="s">
+        <v>174</v>
+      </c>
+      <c r="C26" t="s">
+        <v>172</v>
+      </c>
+      <c r="D26" t="s">
+        <v>130</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="F26">
+        <v>0.95</v>
+      </c>
+      <c r="G26">
+        <v>10</v>
+      </c>
+      <c r="H26">
+        <f>F26*G26</f>
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" t="s">
+        <v>173</v>
+      </c>
+      <c r="C27" t="s">
+        <v>172</v>
+      </c>
+      <c r="D27" t="s">
+        <v>130</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="F27">
+        <v>4.95</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="0"/>
+        <v>4.95</v>
+      </c>
+      <c r="I27" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -1124,9 +1740,28 @@
     <hyperlink ref="B4" r:id="rId4" location="8305a12/=11i0icf"/>
     <hyperlink ref="B5" r:id="rId5" location="92745a320/=11in8yp"/>
     <hyperlink ref="B6" r:id="rId6" location="90272a106/=11indgx"/>
+    <hyperlink ref="E8" r:id="rId7"/>
+    <hyperlink ref="E10" r:id="rId8"/>
+    <hyperlink ref="E11" r:id="rId9"/>
+    <hyperlink ref="E12" r:id="rId10"/>
+    <hyperlink ref="E13" r:id="rId11"/>
+    <hyperlink ref="E14" r:id="rId12"/>
+    <hyperlink ref="E15" r:id="rId13"/>
+    <hyperlink ref="E16" r:id="rId14"/>
+    <hyperlink ref="E17" r:id="rId15"/>
+    <hyperlink ref="E18" r:id="rId16"/>
+    <hyperlink ref="E20" r:id="rId17"/>
+    <hyperlink ref="E19" r:id="rId18"/>
+    <hyperlink ref="E21" r:id="rId19"/>
+    <hyperlink ref="E22" r:id="rId20"/>
+    <hyperlink ref="E23" r:id="rId21"/>
+    <hyperlink ref="E26" r:id="rId22"/>
+    <hyperlink ref="E27" r:id="rId23"/>
+    <hyperlink ref="E25" r:id="rId24"/>
+    <hyperlink ref="E24" r:id="rId25"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId7"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId26"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Fixed routing issues and updated BOM
</commit_message>
<xml_diff>
--- a/design/AGSE_BOM.xlsx
+++ b/design/AGSE_BOM.xlsx
@@ -427,10 +427,10 @@
     <t>http://www.mouser.com/ds/2/307/a165e_ds_e_7_2_csm1264-795350.pdf</t>
   </si>
   <si>
-    <t>A165E-01</t>
-  </si>
-  <si>
     <t>SPST</t>
+  </si>
+  <si>
+    <t>A165E-S-01</t>
   </si>
 </sst>
 </file>
@@ -887,8 +887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1075,7 +1075,7 @@
         <v>130</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C7" t="s">
         <v>17</v>
@@ -1087,17 +1087,17 @@
         <v>132</v>
       </c>
       <c r="F7">
-        <v>20.87</v>
+        <v>32</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>20.87</v>
+        <v>32</v>
       </c>
       <c r="I7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added fuses to bom
</commit_message>
<xml_diff>
--- a/design/AGSE_BOM.xlsx
+++ b/design/AGSE_BOM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hardware" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="137">
   <si>
     <t>Manufacturer Number</t>
   </si>
@@ -355,9 +355,6 @@
     <t>Cartridge Fuses FST 5X20 250V 2A</t>
   </si>
   <si>
-    <t>http://www.mouser.com/ProductDetail/Schurter/00343120/?qs=sGAEpiMZZMtxU2g%2f1juGqbdCHRI5TALuTEcwyPuzfR4%3d</t>
-  </si>
-  <si>
     <t>Fuse Holder</t>
   </si>
   <si>
@@ -431,6 +428,15 @@
   </si>
   <si>
     <t>A165E-S-01</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Littelfuse/0217002MXP/?qs=sGAEpiMZZMtxU2g%2f1juGqbdCHRI5TALuY7Y4dZG08Qk%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Littelfuse/0235003HXP/?qs=sGAEpiMZZMtxU2g%2f1juGqbdCHRI5TALupREhglK8MjI%3d</t>
+  </si>
+  <si>
+    <t>Cartridge Fuses FST 5X20 250V 3A</t>
   </si>
 </sst>
 </file>
@@ -887,7 +893,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -1018,16 +1024,16 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>125</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F5">
         <v>12.6</v>
@@ -1040,21 +1046,21 @@
         <v>12.6</v>
       </c>
       <c r="I5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>129</v>
       </c>
       <c r="C6" t="s">
         <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F6">
         <v>1.46</v>
@@ -1072,19 +1078,19 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C7" t="s">
         <v>17</v>
       </c>
       <c r="D7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>132</v>
       </c>
       <c r="F7">
         <v>32</v>
@@ -1097,7 +1103,7 @@
         <v>32</v>
       </c>
       <c r="I7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1173,10 +1179,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1206,7 +1212,7 @@
     </row>
     <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
         <v>101</v>
@@ -1223,7 +1229,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B3" t="s">
         <v>101</v>
@@ -1249,27 +1255,38 @@
         <v>108</v>
       </c>
       <c r="D4">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>109</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>113</v>
+      <c r="C5" s="10" t="s">
+        <v>136</v>
       </c>
       <c r="D5">
         <v>3</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1277,7 +1294,7 @@
     <hyperlink ref="E2" r:id="rId1"/>
     <hyperlink ref="E3" r:id="rId2"/>
     <hyperlink ref="E4" r:id="rId3"/>
-    <hyperlink ref="E5" r:id="rId4"/>
+    <hyperlink ref="E6" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1384,7 +1401,7 @@
         <v>10</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1459,16 +1476,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>116</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>117</v>
       </c>
       <c r="D11" s="6">
         <v>10</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1645,16 +1662,16 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C31" s="6" t="s">
         <v>119</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>120</v>
       </c>
       <c r="D31" s="6">
         <v>50</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1662,16 +1679,16 @@
         <v>92</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D33" s="6">
         <v>10</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Optimized BOM Quantities for bulk pricing
</commit_message>
<xml_diff>
--- a/design/AGSE_BOM.xlsx
+++ b/design/AGSE_BOM.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hardware" sheetId="1" r:id="rId1"/>
-    <sheet name="Fuse_Board" sheetId="3" r:id="rId2"/>
-    <sheet name="Arm_Motor_Controller" sheetId="2" r:id="rId3"/>
+    <sheet name="PCB_Boards" sheetId="4" r:id="rId2"/>
+    <sheet name="Fuse_Board" sheetId="3" r:id="rId3"/>
+    <sheet name="Arm_Motor_Controller" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027" iterateDelta="1E-4"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="235">
   <si>
     <t>Manufacturer Number</t>
   </si>
@@ -704,13 +705,43 @@
   </si>
   <si>
     <t>http://www.mouser.com/ProductDetail/Schurter/00341521/?qs=sGAEpiMZZMtxU2g%2f1juGqbdCHRI5TALuM6uv50u%252b5gQ%3d</t>
+  </si>
+  <si>
+    <t>Part #</t>
+  </si>
+  <si>
+    <t>Rev</t>
+  </si>
+  <si>
+    <t>Unit Cost</t>
+  </si>
+  <si>
+    <t>Shipping</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Order #</t>
+  </si>
+  <si>
+    <t>MTRBRD</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>FUSEBRD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -764,6 +795,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -811,13 +849,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyProtection="0"/>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
@@ -838,9 +877,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
+    <cellStyle name="Currency" xfId="4" builtinId="4"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="TableStyleLight1" xfId="3"/>
@@ -1157,9 +1200,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1443,10 +1484,96 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1057750</v>
+      </c>
+      <c r="B2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D2" s="11">
+        <v>33</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2" s="11">
+        <v>32.72</v>
+      </c>
+      <c r="G2" s="11">
+        <f>F2+E2*D2</f>
+        <v>164.72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>10577545</v>
+      </c>
+      <c r="B3" t="s">
+        <v>234</v>
+      </c>
+      <c r="C3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D3" s="11">
+        <v>33</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" s="11">
+        <v>32.72</v>
+      </c>
+      <c r="G3" s="12">
+        <f>F3+E3*D3</f>
+        <v>98.72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1509,7 +1636,7 @@
         <v>5.74</v>
       </c>
       <c r="J2">
-        <f t="shared" ref="J2:J7" si="0">H2*D2</f>
+        <f t="shared" ref="J2:J6" si="0">H2*D2</f>
         <v>11.48</v>
       </c>
     </row>
@@ -1641,11 +1768,11 @@
         <v>134</v>
       </c>
       <c r="H8">
-        <v>1.28</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="J8">
         <f t="shared" ref="J8:J27" si="1">H8*D8</f>
-        <v>25.6</v>
+        <v>21.8</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1668,11 +1795,11 @@
         <v>136</v>
       </c>
       <c r="H9">
-        <v>1.1100000000000001</v>
+        <v>0.94699999999999995</v>
       </c>
       <c r="J9">
         <f t="shared" si="1"/>
-        <v>22.200000000000003</v>
+        <v>18.939999999999998</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1686,7 +1813,7 @@
         <v>186</v>
       </c>
       <c r="D10">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>203</v>
@@ -1695,11 +1822,11 @@
         <v>138</v>
       </c>
       <c r="H10">
-        <v>0.13</v>
+        <v>0.04</v>
       </c>
       <c r="J10">
         <f t="shared" si="1"/>
-        <v>7.8000000000000007</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1749,11 +1876,11 @@
         <v>144</v>
       </c>
       <c r="H12">
-        <v>0.42</v>
+        <v>0.33400000000000002</v>
       </c>
       <c r="J12">
         <f t="shared" si="1"/>
-        <v>6.72</v>
+        <v>5.3440000000000003</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1776,11 +1903,11 @@
         <v>146</v>
       </c>
       <c r="H13">
-        <v>0.7</v>
+        <v>0.55100000000000005</v>
       </c>
       <c r="J13">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>5.5100000000000007</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1803,11 +1930,11 @@
         <v>148</v>
       </c>
       <c r="H14">
-        <v>0.1</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="J14">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1830,11 +1957,11 @@
         <v>151</v>
       </c>
       <c r="H15">
-        <v>0.47</v>
+        <v>0.32300000000000001</v>
       </c>
       <c r="J15">
         <f t="shared" si="1"/>
-        <v>7.05</v>
+        <v>4.8449999999999998</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1857,14 +1984,14 @@
         <v>154</v>
       </c>
       <c r="H16">
-        <v>0.36</v>
+        <v>0.193</v>
       </c>
       <c r="J16">
         <f t="shared" si="1"/>
-        <v>5.3999999999999995</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2.895</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>155</v>
       </c>
@@ -1884,14 +2011,14 @@
         <v>157</v>
       </c>
       <c r="H17">
-        <v>0.28999999999999998</v>
+        <v>0.12</v>
       </c>
       <c r="J17">
         <f t="shared" si="1"/>
-        <v>4.3499999999999996</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1.7999999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>158</v>
       </c>
@@ -1911,14 +2038,14 @@
         <v>160</v>
       </c>
       <c r="H18">
-        <v>0.1</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="J18">
         <f t="shared" si="1"/>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.105</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>161</v>
       </c>
@@ -1938,14 +2065,14 @@
         <v>163</v>
       </c>
       <c r="H19">
-        <v>0.49</v>
+        <v>0.35599999999999998</v>
       </c>
       <c r="J19">
         <f t="shared" si="1"/>
-        <v>14.7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+        <v>10.68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>164</v>
       </c>
@@ -1965,14 +2092,14 @@
         <v>163</v>
       </c>
       <c r="H20">
-        <v>0.48</v>
+        <v>0.28199999999999997</v>
       </c>
       <c r="J20">
         <f t="shared" si="1"/>
-        <v>14.399999999999999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+        <v>8.4599999999999991</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>166</v>
       </c>
@@ -1992,14 +2119,14 @@
         <v>168</v>
       </c>
       <c r="H21">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="J21">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>169</v>
       </c>
@@ -2019,14 +2146,14 @@
         <v>168</v>
       </c>
       <c r="H22">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="J22">
         <f t="shared" si="1"/>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>171</v>
       </c>
@@ -2037,7 +2164,7 @@
         <v>196</v>
       </c>
       <c r="D23">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>215</v>
@@ -2046,14 +2173,14 @@
         <v>173</v>
       </c>
       <c r="H23">
-        <v>0.1</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="J23">
         <f t="shared" si="1"/>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>174</v>
       </c>
@@ -2073,14 +2200,14 @@
         <v>176</v>
       </c>
       <c r="H24">
-        <v>0.23</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="J24">
         <f t="shared" si="1"/>
-        <v>2.3000000000000003</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>177</v>
       </c>
@@ -2100,14 +2227,14 @@
         <v>179</v>
       </c>
       <c r="H25">
-        <v>0.71</v>
+        <v>0.52900000000000003</v>
       </c>
       <c r="J25">
         <f t="shared" si="1"/>
-        <v>7.1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+        <v>5.29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>117</v>
       </c>
@@ -2134,7 +2261,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>50</v>
       </c>
@@ -2161,10 +2288,13 @@
         <v>4.95</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="J30">
         <f>SUM(J2:J28)</f>
-        <v>193.10999999999999</v>
+        <v>155.93899999999999</v>
+      </c>
+      <c r="M30">
+        <v>193.11</v>
       </c>
     </row>
   </sheetData>
@@ -2225,7 +2355,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F36"/>
   <sheetViews>

</xml_diff>